<commit_message>
Mise à jour du fichier Portfolio et ajout de la présentation finale
</commit_message>
<xml_diff>
--- a/Portfolio.xlsx
+++ b/Portfolio.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathi\Desktop\Cours et Exam BTS\Portfolio E5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202D8348-EC07-421A-8B50-99E04CD6708C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BA4E45E-77A6-4080-B2C7-6033DC71FDB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="50">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -112,9 +112,6 @@
     <t>NOM et prénom : KOVACEVIC Mathieu</t>
   </si>
   <si>
-    <t>Centre de formation : Studi</t>
-  </si>
-  <si>
     <t>Adresse URL du portfolio : https://github.com/MathieuKovacevic/</t>
   </si>
   <si>
@@ -183,6 +180,18 @@
   <si>
     <t xml:space="preserve">Réalisations en cours de formation
 </t>
+  </si>
+  <si>
+    <t>Installation et configuration d'un pare-feu (Pfsense)</t>
+  </si>
+  <si>
+    <t>Centre de formation : STUDI</t>
+  </si>
+  <si>
+    <t>Réalisation d'un cahier des charges</t>
+  </si>
+  <si>
+    <t>Mise en place du portfolio</t>
   </si>
 </sst>
 </file>
@@ -716,15 +725,39 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -756,30 +789,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1092,8 +1101,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1106,56 +1115,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="23"/>
+      <c r="H1" s="21"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="41" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="36"/>
-      <c r="H3" s="42"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="23"/>
+      <c r="H3" s="29"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="40"/>
+      <c r="A4" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="27"/>
       <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
@@ -1167,22 +1176,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34"/>
+      <c r="A5" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="42"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="30" t="s">
+      <c r="B6" s="38" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1205,8 +1214,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="31"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1262,16 +1271,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
+      <c r="A8" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1310,24 +1319,24 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="10">
         <v>2024</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="17"/>
       <c r="E9" s="17"/>
       <c r="F9" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H9" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
@@ -1367,7 +1376,7 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" s="10">
         <v>2024</v>
@@ -1376,10 +1385,10 @@
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H10" s="19"/>
       <c r="I10"/>
@@ -1420,18 +1429,18 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="10">
         <v>2024</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="17"/>
       <c r="F11" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="19"/>
@@ -1473,18 +1482,18 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B12" s="10">
         <v>2025</v>
       </c>
       <c r="C12" s="17"/>
       <c r="D12" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E12" s="17"/>
       <c r="F12" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="19"/>
@@ -1526,7 +1535,7 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="10">
         <v>2025</v>
@@ -1535,11 +1544,11 @@
       <c r="D13" s="17"/>
       <c r="E13" s="17"/>
       <c r="F13" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I13"/>
       <c r="J13"/>
@@ -1579,26 +1588,26 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B14" s="10">
         <v>2025</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="17"/>
       <c r="F14" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H14" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I14"/>
       <c r="J14"/>
@@ -1638,20 +1647,20 @@
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="10">
         <v>2025</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
       <c r="H15" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I15"/>
       <c r="J15"/>
@@ -1690,13 +1699,21 @@
       <c r="AQ15"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11"/>
-      <c r="B16" s="10"/>
+      <c r="A16" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="10">
+        <v>2025</v>
+      </c>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
+      <c r="F16" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="H16" s="19"/>
       <c r="I16"/>
       <c r="J16"/>
@@ -1735,9 +1752,15 @@
       <c r="AQ16"/>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="17"/>
+      <c r="A17" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="10">
+        <v>2025</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="D17" s="17"/>
       <c r="E17" s="17"/>
       <c r="F17" s="17"/>
@@ -1780,14 +1803,20 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11"/>
+      <c r="A18" s="11" t="s">
+        <v>49</v>
+      </c>
       <c r="B18" s="10"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="19"/>
+      <c r="G18" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>42</v>
+      </c>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1825,16 +1854,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="29"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="37"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1873,26 +1902,26 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B20" s="10">
         <v>2020</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E20" s="17"/>
       <c r="F20" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I20"/>
       <c r="J20"/>
@@ -1932,21 +1961,21 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="10">
         <v>2020</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="17"/>
       <c r="G21" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H21" s="19"/>
       <c r="I21"/>
@@ -1987,21 +2016,21 @@
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="10">
         <v>2020</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
       <c r="G22" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H22" s="19"/>
       <c r="I22"/>
@@ -2042,23 +2071,23 @@
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="10">
         <v>2020</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E23" s="17"/>
       <c r="F23" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H23" s="19"/>
       <c r="I23"/>
@@ -2099,19 +2128,19 @@
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="10">
         <v>2021</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
       <c r="G24" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H24" s="19"/>
       <c r="I24"/>
@@ -2152,7 +2181,7 @@
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="10">
         <v>2021</v>
@@ -2160,10 +2189,10 @@
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="19"/>
@@ -2249,16 +2278,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A27" s="27" t="s">
+      <c r="A27" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="29"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="37"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2297,24 +2326,24 @@
     </row>
     <row r="28" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="10">
         <v>2024</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D28" s="17"/>
       <c r="E28" s="17"/>
       <c r="F28" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H28" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I28"/>
       <c r="J28"/>
@@ -2354,18 +2383,18 @@
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" s="10">
         <v>2024</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D29" s="17"/>
       <c r="E29" s="17"/>
       <c r="F29" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="19"/>
@@ -2407,23 +2436,23 @@
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="10">
         <v>2024</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E30" s="17"/>
       <c r="F30" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G30" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H30" s="19"/>
       <c r="I30"/>
@@ -2464,16 +2493,16 @@
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="10">
         <v>2024</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="17"/>
@@ -2517,22 +2546,22 @@
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" s="10">
         <v>2025</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D32" s="17"/>
       <c r="E32" s="17"/>
       <c r="F32" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G32" s="17"/>
       <c r="H32" s="19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I32"/>
       <c r="J32"/>
@@ -2572,23 +2601,23 @@
     </row>
     <row r="33" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B33" s="10">
         <v>2025</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E33" s="17"/>
       <c r="F33" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H33" s="19"/>
       <c r="I33"/>
@@ -2628,12 +2657,20 @@
       <c r="AQ33"/>
     </row>
     <row r="34" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
-      <c r="B34" s="13"/>
+      <c r="A34" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="13">
+        <v>2025</v>
+      </c>
       <c r="C34" s="18"/>
       <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18"/>
+      <c r="E34" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>42</v>
+      </c>
       <c r="G34" s="18"/>
       <c r="H34" s="20"/>
       <c r="I34"/>
@@ -2765,11 +2802,6 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2777,6 +2809,11 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>